<commit_message>
revisiting mistnet data to share with TTinker
</commit_message>
<xml_diff>
--- a/ASSP_share/mistnetting_CPUE_2017-2018.xlsx
+++ b/ASSP_share/mistnetting_CPUE_2017-2018.xlsx
@@ -16,14 +16,14 @@
     <sheet name="definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CPUE_2017-2018'!$A$1:$Z$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CPUE_2017-2018'!$A$1:$AC$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="153">
   <si>
     <t>island</t>
   </si>
@@ -443,6 +443,45 @@
   </si>
   <si>
     <t>Mistnetting sites at the five islands listed above.  See 'ASSP_mistnetting_locs_20190905.csv' for discription</t>
+  </si>
+  <si>
+    <t>seq_night</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>sequental mistnetting night: 1 = first/only night, 2 = 2nd night in a row, 3 = 3rd night in a row</t>
+  </si>
+  <si>
+    <t>SPID</t>
+  </si>
+  <si>
+    <t>songmeter ID of the closest SM to the netting site</t>
+  </si>
+  <si>
+    <t>PI_AB47</t>
+  </si>
+  <si>
+    <t>PI_CP</t>
+  </si>
+  <si>
+    <t>SBI_AP</t>
+  </si>
+  <si>
+    <t>SBI_ESP</t>
+  </si>
+  <si>
+    <t>SR_A</t>
+  </si>
+  <si>
+    <t>PI_AB47, PI_CP, SBI_AP, SBI_CC, SBI_ESP, SBI_LC, SR_A</t>
+  </si>
+  <si>
+    <t>SPID_2</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -937,11 +976,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -955,6 +992,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1276,2942 +1318,3268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="3"/>
+    <col min="10" max="10" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.140625" style="3"/>
+    <col min="19" max="19" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="32" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="10">
         <v>42880</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
         <v>33.487622000000002</v>
       </c>
-      <c r="F2">
+      <c r="I2" s="3">
         <v>-119.02853500000001</v>
       </c>
-      <c r="G2" s="1">
+      <c r="J2" s="11">
         <v>42880.831921296296</v>
       </c>
-      <c r="H2">
+      <c r="K2" s="3">
         <v>1.79865002181367E-3</v>
       </c>
-      <c r="I2">
+      <c r="L2" s="3">
         <v>453</v>
       </c>
-      <c r="J2">
+      <c r="M2" s="3">
         <v>0.81478845988159398</v>
       </c>
-      <c r="K2" s="1">
+      <c r="N2" s="11">
         <v>42880.892361111109</v>
       </c>
-      <c r="L2" s="1">
+      <c r="O2" s="11">
         <v>42881.083333333336</v>
       </c>
-      <c r="M2" s="1">
+      <c r="P2" s="11">
         <v>42881.052754629629</v>
       </c>
-      <c r="N2">
+      <c r="Q2" s="3">
         <v>275</v>
       </c>
-      <c r="O2">
+      <c r="R2" s="3">
         <v>230</v>
       </c>
-      <c r="P2">
+      <c r="S2" s="3">
         <v>14</v>
       </c>
-      <c r="Q2">
+      <c r="T2" s="3">
         <v>13</v>
       </c>
-      <c r="R2">
+      <c r="U2" s="3">
         <v>5.0909090909090897E-2</v>
       </c>
-      <c r="S2">
+      <c r="V2" s="3">
         <v>5.6521739130434803E-2</v>
       </c>
-      <c r="T2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="W2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AB2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AC2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="10">
         <v>42908</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
         <v>33.487622000000002</v>
       </c>
-      <c r="F3">
+      <c r="I3" s="3">
         <v>-119.02853500000001</v>
       </c>
-      <c r="G3" s="1">
+      <c r="J3" s="11">
         <v>42908.840729166666</v>
       </c>
-      <c r="H3">
+      <c r="K3" s="3">
         <v>2.4698168643905099E-2</v>
       </c>
-      <c r="I3">
+      <c r="L3" s="3">
         <v>440</v>
       </c>
-      <c r="J3">
+      <c r="M3" s="3">
         <v>10.8671942033183</v>
       </c>
-      <c r="K3" s="1">
+      <c r="N3" s="11">
         <v>42908.854166666664</v>
       </c>
-      <c r="L3" s="1">
+      <c r="O3" s="11">
         <v>42909.083333333336</v>
       </c>
-      <c r="M3" s="1">
+      <c r="P3" s="11">
         <v>42909.061562499999</v>
       </c>
-      <c r="N3">
+      <c r="Q3" s="3">
         <v>330</v>
       </c>
-      <c r="O3">
+      <c r="R3" s="3">
         <v>298</v>
       </c>
-      <c r="P3">
+      <c r="S3" s="3">
         <v>25</v>
       </c>
-      <c r="Q3">
+      <c r="T3" s="3">
         <v>22</v>
       </c>
-      <c r="R3">
+      <c r="U3" s="3">
         <v>7.5757575757575801E-2</v>
       </c>
-      <c r="S3">
+      <c r="V3" s="3">
         <v>7.3825503355704702E-2</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="10">
         <v>43232</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
         <v>33.487622000000002</v>
       </c>
-      <c r="F4">
+      <c r="I4" s="3">
         <v>-119.02853500000001</v>
       </c>
-      <c r="G4" s="1">
+      <c r="J4" s="11">
         <v>43232.825266203705</v>
       </c>
-      <c r="H4">
+      <c r="K4" s="3">
         <v>9.7866366256189899E-2</v>
       </c>
-      <c r="I4">
+      <c r="L4" s="3">
         <v>698</v>
       </c>
-      <c r="J4">
+      <c r="M4" s="3">
         <v>68.310723646820605</v>
       </c>
-      <c r="K4" s="1">
+      <c r="N4" s="11">
         <v>43232.871527777781</v>
       </c>
-      <c r="L4" s="1">
+      <c r="O4" s="11">
         <v>43233.090277777781</v>
       </c>
-      <c r="M4" s="1">
+      <c r="P4" s="11">
         <v>43233.046099537038</v>
       </c>
-      <c r="N4">
+      <c r="Q4" s="3">
         <v>315</v>
       </c>
-      <c r="O4">
+      <c r="R4" s="3">
         <v>251</v>
       </c>
-      <c r="P4">
-        <v>29</v>
-      </c>
-      <c r="Q4">
+      <c r="S4" s="3">
+        <v>29</v>
+      </c>
+      <c r="T4" s="3">
         <v>22</v>
       </c>
-      <c r="R4">
+      <c r="U4" s="3">
         <v>9.2063492063492097E-2</v>
       </c>
-      <c r="S4">
+      <c r="V4" s="3">
         <v>8.7649402390438294E-2</v>
       </c>
-      <c r="T4" t="s">
+      <c r="W4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U4" t="s">
+      <c r="X4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V4" t="s">
+      <c r="Y4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Z4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AA4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AB4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AC4" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="10">
         <v>43261</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
         <v>33.487622000000002</v>
       </c>
-      <c r="F5">
+      <c r="I5" s="3">
         <v>-119.02853500000001</v>
       </c>
-      <c r="G5" s="1">
+      <c r="J5" s="11">
         <v>43261.838101851848</v>
       </c>
-      <c r="H5">
+      <c r="K5" s="3">
         <v>0.12540511530571</v>
       </c>
-      <c r="I5">
+      <c r="L5" s="3">
         <v>601</v>
       </c>
-      <c r="J5">
+      <c r="M5" s="3">
         <v>75.368474298731996</v>
       </c>
-      <c r="K5" s="1">
+      <c r="N5" s="11">
         <v>43261.916666666664</v>
       </c>
-      <c r="L5" s="1">
+      <c r="O5" s="11">
         <v>43262.125</v>
       </c>
-      <c r="M5" s="1">
+      <c r="P5" s="11">
         <v>43262.058935185189</v>
       </c>
-      <c r="N5">
+      <c r="Q5" s="3">
         <v>290</v>
       </c>
-      <c r="O5">
+      <c r="R5" s="3">
         <v>194</v>
       </c>
-      <c r="P5">
+      <c r="S5" s="3">
         <v>33</v>
       </c>
-      <c r="Q5">
+      <c r="T5" s="3">
         <v>23</v>
       </c>
-      <c r="R5">
+      <c r="U5" s="3">
         <v>0.11379310344827601</v>
       </c>
-      <c r="S5">
+      <c r="V5" s="3">
         <v>0.118556701030928</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V5" t="s">
+      <c r="Y5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Z5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AA5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AB5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AC5" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="10">
         <v>43289</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
         <v>33.487622000000002</v>
       </c>
-      <c r="F6">
+      <c r="I6" s="3">
         <v>-119.02853500000001</v>
       </c>
-      <c r="G6" s="1">
+      <c r="J6" s="11">
         <v>43289.840439814812</v>
       </c>
-      <c r="H6">
+      <c r="K6" s="3">
         <v>0.25413669520403198</v>
       </c>
-      <c r="I6">
+      <c r="L6" s="3">
         <v>564</v>
       </c>
-      <c r="J6">
+      <c r="M6" s="3">
         <v>143.33309609507401</v>
       </c>
-      <c r="K6" s="1">
+      <c r="N6" s="11">
         <v>43289.875</v>
       </c>
-      <c r="L6" s="1">
+      <c r="O6" s="11">
         <v>43290.045138888891</v>
       </c>
-      <c r="M6" s="1">
+      <c r="P6" s="11">
         <v>43290.061273148145</v>
       </c>
-      <c r="N6">
+      <c r="Q6" s="3">
         <v>235</v>
       </c>
-      <c r="O6">
+      <c r="R6" s="3">
         <v>235</v>
       </c>
-      <c r="P6">
+      <c r="S6" s="3">
         <v>19</v>
       </c>
-      <c r="Q6">
+      <c r="T6" s="3">
         <v>19</v>
       </c>
-      <c r="R6">
+      <c r="U6" s="3">
         <v>8.0851063829787198E-2</v>
       </c>
-      <c r="S6">
+      <c r="V6" s="3">
         <v>8.0851063829787198E-2</v>
       </c>
-      <c r="T6" t="s">
+      <c r="W6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U6" t="s">
+      <c r="X6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V6" t="s">
+      <c r="Y6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Z6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X6" t="s">
+      <c r="AA6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AB6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AC6" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="10">
         <v>43325</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
         <v>33.487622000000002</v>
       </c>
-      <c r="F7">
+      <c r="I7" s="3">
         <v>-119.02853500000001</v>
       </c>
-      <c r="G7" s="1">
+      <c r="J7" s="11">
         <v>43325.823761574073</v>
       </c>
-      <c r="H7">
+      <c r="K7" s="3">
         <v>6.6903978821831106E-2</v>
       </c>
-      <c r="I7">
+      <c r="L7" s="3">
         <v>580</v>
       </c>
-      <c r="J7">
+      <c r="M7" s="3">
         <v>38.804307716662002</v>
       </c>
-      <c r="K7" s="1">
+      <c r="N7" s="11">
         <v>43325.881944444445</v>
       </c>
-      <c r="L7" s="1">
+      <c r="O7" s="11">
         <v>43326.090277777781</v>
       </c>
-      <c r="M7" s="1">
+      <c r="P7" s="11">
         <v>43326.044594907406</v>
       </c>
-      <c r="N7">
+      <c r="Q7" s="3">
         <v>300</v>
       </c>
-      <c r="O7">
+      <c r="R7" s="3">
         <v>234</v>
       </c>
-      <c r="P7">
+      <c r="S7" s="3">
         <v>10</v>
       </c>
-      <c r="Q7">
+      <c r="T7" s="3">
         <v>3</v>
       </c>
-      <c r="R7">
+      <c r="U7" s="3">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="S7">
+      <c r="V7" s="3">
         <v>1.2820512820512799E-2</v>
       </c>
-      <c r="T7" t="s">
+      <c r="W7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U7" t="s">
+      <c r="X7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V7" t="s">
+      <c r="Y7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Z7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X7" t="s">
+      <c r="AA7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AB7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AC7" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="10">
         <v>43326</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3">
         <v>33.487622000000002</v>
       </c>
-      <c r="F8">
+      <c r="I8" s="3">
         <v>-119.02853500000001</v>
       </c>
-      <c r="G8" s="1">
+      <c r="J8" s="11">
         <v>43326.823020833333</v>
       </c>
-      <c r="H8">
+      <c r="K8" s="3">
         <v>0.13216562844208399</v>
       </c>
-      <c r="I8">
+      <c r="L8" s="3">
         <v>660</v>
       </c>
-      <c r="J8">
+      <c r="M8" s="3">
         <v>87.229314771775293</v>
       </c>
-      <c r="K8" s="1">
+      <c r="N8" s="11">
         <v>43326.880555555559</v>
       </c>
-      <c r="L8" s="1">
+      <c r="O8" s="11">
         <v>43327.076388888891</v>
       </c>
-      <c r="M8" s="1">
+      <c r="P8" s="11">
         <v>43327.043854166666</v>
       </c>
-      <c r="N8">
+      <c r="Q8" s="3">
         <v>282</v>
       </c>
-      <c r="O8">
+      <c r="R8" s="3">
         <v>235</v>
       </c>
-      <c r="P8">
+      <c r="S8" s="3">
         <v>7</v>
       </c>
-      <c r="Q8">
+      <c r="T8" s="3">
         <v>5</v>
       </c>
-      <c r="R8">
+      <c r="U8" s="3">
         <v>2.4822695035461001E-2</v>
       </c>
-      <c r="S8">
+      <c r="V8" s="3">
         <v>2.1276595744680899E-2</v>
       </c>
-      <c r="T8" t="s">
+      <c r="W8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U8" t="s">
+      <c r="X8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V8" t="s">
+      <c r="Y8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Z8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X8" t="s">
+      <c r="AA8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AB8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AC8" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="10">
         <v>42881</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
         <v>33.482528000000002</v>
       </c>
-      <c r="F9">
+      <c r="I9" s="3">
         <v>-119.04159900000001</v>
       </c>
-      <c r="G9" s="1">
+      <c r="J9" s="11">
         <v>42881.832407407404</v>
       </c>
-      <c r="H9">
+      <c r="K9" s="3">
         <v>1.3276466411268501E-2</v>
       </c>
-      <c r="I9">
+      <c r="L9" s="3">
         <v>399</v>
       </c>
-      <c r="J9">
+      <c r="M9" s="3">
         <v>5.2973100980961298</v>
       </c>
-      <c r="K9" s="1">
+      <c r="N9" s="11">
         <v>42881.875</v>
       </c>
-      <c r="L9" s="1">
+      <c r="O9" s="11">
         <v>42882.083333333336</v>
       </c>
-      <c r="M9" s="1">
+      <c r="P9" s="11">
         <v>42882.053240740737</v>
       </c>
-      <c r="N9">
+      <c r="Q9" s="3">
         <v>300</v>
       </c>
-      <c r="O9">
+      <c r="R9" s="3">
         <v>256</v>
       </c>
-      <c r="P9">
+      <c r="S9" s="3">
         <v>27</v>
       </c>
-      <c r="Q9">
+      <c r="T9" s="3">
         <v>25</v>
       </c>
-      <c r="R9">
+      <c r="U9" s="3">
         <v>0.09</v>
       </c>
-      <c r="S9">
+      <c r="V9" s="3">
         <v>9.765625E-2</v>
       </c>
-      <c r="T9" t="s">
-        <v>29</v>
-      </c>
-      <c r="U9" t="s">
+      <c r="W9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V9" t="s">
+      <c r="Y9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W9" t="s">
+      <c r="Z9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X9" t="s">
+      <c r="AA9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AB9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AC9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="10">
         <v>43233</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
         <v>33.482528000000002</v>
       </c>
-      <c r="F10">
+      <c r="I10" s="3">
         <v>-119.04159900000001</v>
       </c>
-      <c r="G10" s="1">
+      <c r="J10" s="11">
         <v>43233.825821759259</v>
       </c>
-      <c r="H10">
+      <c r="K10" s="3">
         <v>4.2567938432832103E-2</v>
       </c>
-      <c r="I10">
+      <c r="L10" s="3">
         <v>623</v>
       </c>
-      <c r="J10">
+      <c r="M10" s="3">
         <v>26.5198256436544</v>
       </c>
-      <c r="K10" s="1">
+      <c r="N10" s="11">
         <v>43233.86041666667</v>
       </c>
-      <c r="L10" s="1">
+      <c r="O10" s="11">
         <v>43234.086805555555</v>
       </c>
-      <c r="M10" s="1">
+      <c r="P10" s="11">
         <v>43234.046655092592</v>
       </c>
-      <c r="N10">
+      <c r="Q10" s="3">
         <v>326</v>
       </c>
-      <c r="O10">
+      <c r="R10" s="3">
         <v>268</v>
       </c>
-      <c r="P10">
+      <c r="S10" s="3">
         <v>35</v>
       </c>
-      <c r="Q10">
-        <v>29</v>
-      </c>
-      <c r="R10">
+      <c r="T10" s="3">
+        <v>29</v>
+      </c>
+      <c r="U10" s="3">
         <v>0.107361963190184</v>
       </c>
-      <c r="S10">
+      <c r="V10" s="3">
         <v>0.10820895522388101</v>
       </c>
-      <c r="T10" t="s">
+      <c r="W10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U10" t="s">
+      <c r="X10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V10" t="s">
+      <c r="Y10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W10" t="s">
+      <c r="Z10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X10" t="s">
+      <c r="AA10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AB10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AC10" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="10">
         <v>43262</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
         <v>33.482528000000002</v>
       </c>
-      <c r="F11">
+      <c r="I11" s="3">
         <v>-119.04159900000001</v>
       </c>
-      <c r="G11" s="1">
+      <c r="J11" s="11">
         <v>43262.838425925926</v>
       </c>
-      <c r="H11">
+      <c r="K11" s="3">
         <v>5.7589354030415298E-2</v>
       </c>
-      <c r="I11">
+      <c r="L11" s="3">
         <v>517</v>
       </c>
-      <c r="J11">
+      <c r="M11" s="3">
         <v>29.773696033724701</v>
       </c>
-      <c r="K11" s="1">
+      <c r="N11" s="11">
         <v>43262.877083333333</v>
       </c>
-      <c r="L11" s="1">
+      <c r="O11" s="11">
         <v>43263.083333333336</v>
       </c>
-      <c r="M11" s="1">
+      <c r="P11" s="11">
         <v>43263.059259259258</v>
       </c>
-      <c r="N11">
+      <c r="Q11" s="3">
         <v>297</v>
       </c>
-      <c r="O11">
+      <c r="R11" s="3">
         <v>262</v>
       </c>
-      <c r="P11">
+      <c r="S11" s="3">
         <v>40</v>
       </c>
-      <c r="Q11">
+      <c r="T11" s="3">
         <v>39</v>
       </c>
-      <c r="R11">
+      <c r="U11" s="3">
         <v>0.13468013468013501</v>
       </c>
-      <c r="S11">
+      <c r="V11" s="3">
         <v>0.14885496183206101</v>
       </c>
-      <c r="T11" t="s">
+      <c r="W11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U11" t="s">
+      <c r="X11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V11" t="s">
+      <c r="Y11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W11" t="s">
+      <c r="Z11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X11" t="s">
+      <c r="AA11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AB11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AC11" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="10">
         <v>43287</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
         <v>33.482528000000002</v>
       </c>
-      <c r="F12">
+      <c r="I12" s="3">
         <v>-119.04159900000001</v>
       </c>
-      <c r="G12" s="1">
+      <c r="J12" s="11">
         <v>43287.840752314813</v>
       </c>
-      <c r="H12">
+      <c r="K12" s="3">
         <v>0.46742817045948898</v>
       </c>
-      <c r="I12">
+      <c r="L12" s="3">
         <v>704</v>
       </c>
-      <c r="J12">
+      <c r="M12" s="3">
         <v>329.06943200348002</v>
       </c>
-      <c r="K12" s="1">
+      <c r="N12" s="11">
         <v>43287.879166666666</v>
       </c>
-      <c r="L12" s="1">
+      <c r="O12" s="11">
         <v>43288.020138888889</v>
       </c>
-      <c r="M12" s="1">
+      <c r="P12" s="11">
         <v>43288.061585648145</v>
       </c>
-      <c r="N12">
+      <c r="Q12" s="3">
         <v>203</v>
       </c>
-      <c r="O12">
+      <c r="R12" s="3">
         <v>203</v>
       </c>
-      <c r="P12">
+      <c r="S12" s="3">
         <v>19</v>
       </c>
-      <c r="Q12">
+      <c r="T12" s="3">
         <v>19</v>
       </c>
-      <c r="R12">
+      <c r="U12" s="3">
         <v>9.3596059113300503E-2</v>
       </c>
-      <c r="S12">
+      <c r="V12" s="3">
         <v>9.3596059113300503E-2</v>
       </c>
-      <c r="T12" t="s">
+      <c r="W12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U12" t="s">
+      <c r="X12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V12" t="s">
+      <c r="Y12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W12" t="s">
+      <c r="Z12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X12" t="s">
+      <c r="AA12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AB12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AC12" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="10">
         <v>43288</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
         <v>33.482528000000002</v>
       </c>
-      <c r="F13">
+      <c r="I13" s="3">
         <v>-119.04159900000001</v>
       </c>
-      <c r="G13" s="1">
+      <c r="J13" s="11">
         <v>43288.840624999997</v>
       </c>
-      <c r="H13">
+      <c r="K13" s="3">
         <v>0.35940817587200902</v>
       </c>
-      <c r="I13">
+      <c r="L13" s="3">
         <v>634</v>
       </c>
-      <c r="J13">
+      <c r="M13" s="3">
         <v>227.86478350285401</v>
       </c>
-      <c r="K13" s="1">
+      <c r="N13" s="11">
         <v>43288.875</v>
       </c>
-      <c r="L13" s="1">
+      <c r="O13" s="11">
         <v>43289.083333333336</v>
       </c>
-      <c r="M13" s="1">
+      <c r="P13" s="11">
         <v>43289.06145833333</v>
       </c>
-      <c r="N13">
+      <c r="Q13" s="3">
         <v>240</v>
       </c>
-      <c r="O13">
+      <c r="R13" s="3">
         <v>208</v>
       </c>
-      <c r="P13">
+      <c r="S13" s="3">
         <v>27</v>
       </c>
-      <c r="Q13">
+      <c r="T13" s="3">
         <v>23</v>
       </c>
-      <c r="R13">
+      <c r="U13" s="3">
         <v>0.1125</v>
       </c>
-      <c r="S13">
+      <c r="V13" s="3">
         <v>0.110576923076923</v>
       </c>
-      <c r="T13" t="s">
+      <c r="W13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U13" t="s">
+      <c r="X13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V13" t="s">
+      <c r="Y13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W13" t="s">
+      <c r="Z13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X13" t="s">
+      <c r="AA13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AB13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AC13" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="10">
         <v>43327</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
         <v>33.482528000000002</v>
       </c>
-      <c r="F14">
+      <c r="I14" s="3">
         <v>-119.04159900000001</v>
       </c>
-      <c r="G14" s="1">
+      <c r="J14" s="11">
         <v>43327.82230324074</v>
       </c>
-      <c r="H14">
+      <c r="K14" s="3">
         <v>0.21492857696447601</v>
       </c>
-      <c r="I14">
+      <c r="L14" s="3">
         <v>737</v>
       </c>
-      <c r="J14">
+      <c r="M14" s="3">
         <v>158.402361222819</v>
       </c>
-      <c r="K14" s="1">
+      <c r="N14" s="11">
         <v>43327.875</v>
       </c>
-      <c r="L14" s="1">
+      <c r="O14" s="11">
         <v>43328.09097222222</v>
       </c>
-      <c r="M14" s="1">
+      <c r="P14" s="11">
         <v>43328.043136574073</v>
       </c>
-      <c r="N14">
+      <c r="Q14" s="3">
         <v>311</v>
       </c>
-      <c r="O14">
+      <c r="R14" s="3">
         <v>242</v>
       </c>
-      <c r="P14">
+      <c r="S14" s="3">
         <v>13</v>
       </c>
-      <c r="Q14">
+      <c r="T14" s="3">
         <v>9</v>
       </c>
-      <c r="R14">
+      <c r="U14" s="3">
         <v>4.1800643086816698E-2</v>
       </c>
-      <c r="S14">
+      <c r="V14" s="3">
         <v>3.71900826446281E-2</v>
       </c>
-      <c r="T14" t="s">
+      <c r="W14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U14" t="s">
+      <c r="X14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V14" t="s">
+      <c r="Y14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W14" t="s">
+      <c r="Z14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X14" t="s">
+      <c r="AA14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AB14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AC14" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="10">
         <v>43234</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F15">
+      <c r="I15" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G15" s="1">
+      <c r="J15" s="11">
         <v>43234.830752314818</v>
       </c>
-      <c r="H15">
+      <c r="K15" s="3">
         <v>9.7616974305620805E-3</v>
       </c>
-      <c r="I15">
+      <c r="L15" s="3">
         <v>556</v>
       </c>
-      <c r="J15">
+      <c r="M15" s="3">
         <v>5.4275037713925203</v>
       </c>
-      <c r="K15" s="1">
+      <c r="N15" s="11">
         <v>43234.869444444441</v>
       </c>
-      <c r="L15" s="1">
+      <c r="O15" s="11">
         <v>43235.083333333336</v>
       </c>
-      <c r="M15" s="1">
+      <c r="P15" s="11">
         <v>43235.051585648151</v>
       </c>
-      <c r="N15">
+      <c r="Q15" s="3">
         <v>308</v>
       </c>
-      <c r="O15">
+      <c r="R15" s="3">
         <v>262</v>
       </c>
-      <c r="P15">
+      <c r="S15" s="3">
         <v>34</v>
       </c>
-      <c r="Q15">
-        <v>29</v>
-      </c>
-      <c r="R15">
+      <c r="T15" s="3">
+        <v>29</v>
+      </c>
+      <c r="U15" s="3">
         <v>0.11038961038961</v>
       </c>
-      <c r="S15">
+      <c r="V15" s="3">
         <v>0.110687022900763</v>
       </c>
-      <c r="T15" t="s">
-        <v>29</v>
-      </c>
-      <c r="U15" t="s">
-        <v>29</v>
-      </c>
-      <c r="V15" t="s">
-        <v>29</v>
-      </c>
-      <c r="W15" t="s">
-        <v>29</v>
-      </c>
-      <c r="X15" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y15" t="s">
+      <c r="W15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AC15" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="10">
         <v>43235</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F16">
+      <c r="I16" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G16" s="1">
+      <c r="J16" s="11">
         <v>43235.831284722219</v>
       </c>
-      <c r="H16">
+      <c r="K16" s="3">
         <v>2.2487391111391799E-3</v>
       </c>
-      <c r="I16">
+      <c r="L16" s="3">
         <v>486</v>
       </c>
-      <c r="J16">
+      <c r="M16" s="3">
         <v>1.09288720801364</v>
       </c>
-      <c r="K16" s="1">
+      <c r="N16" s="11">
         <v>43235.859722222223</v>
       </c>
-      <c r="L16" s="1">
+      <c r="O16" s="11">
         <v>43236.079861111109</v>
       </c>
-      <c r="M16" s="1">
+      <c r="P16" s="11">
         <v>43236.052118055559</v>
       </c>
-      <c r="N16">
+      <c r="Q16" s="3">
         <v>317</v>
       </c>
-      <c r="O16">
+      <c r="R16" s="3">
         <v>277</v>
       </c>
-      <c r="P16">
+      <c r="S16" s="3">
         <v>13</v>
       </c>
-      <c r="Q16">
+      <c r="T16" s="3">
         <v>10</v>
       </c>
-      <c r="R16">
+      <c r="U16" s="3">
         <v>4.1009463722397499E-2</v>
       </c>
-      <c r="S16">
+      <c r="V16" s="3">
         <v>3.6101083032491002E-2</v>
       </c>
-      <c r="T16" t="s">
-        <v>29</v>
-      </c>
-      <c r="U16" t="s">
-        <v>29</v>
-      </c>
-      <c r="V16" t="s">
-        <v>29</v>
-      </c>
-      <c r="W16" t="s">
-        <v>29</v>
-      </c>
-      <c r="X16" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y16" t="s">
+      <c r="W16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AC16" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="10">
         <v>43262</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F17">
+      <c r="I17" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G17" s="1">
+      <c r="J17" s="11">
         <v>43262.843055555553</v>
       </c>
-      <c r="H17">
+      <c r="K17" s="3">
         <v>5.7745371579358003E-2</v>
       </c>
-      <c r="I17">
+      <c r="L17" s="3">
         <v>525</v>
       </c>
-      <c r="J17">
+      <c r="M17" s="3">
         <v>30.316320079162999</v>
       </c>
-      <c r="K17" s="1">
+      <c r="N17" s="11">
         <v>43262.881249999999</v>
       </c>
-      <c r="L17" s="1">
+      <c r="O17" s="11">
         <v>43263.083333333336</v>
       </c>
-      <c r="M17" s="1">
+      <c r="P17" s="11">
         <v>43263.063888888886</v>
       </c>
-      <c r="N17">
+      <c r="Q17" s="3">
         <v>291</v>
       </c>
-      <c r="O17">
+      <c r="R17" s="3">
         <v>263</v>
       </c>
-      <c r="P17">
+      <c r="S17" s="3">
         <v>18</v>
       </c>
-      <c r="Q17">
+      <c r="T17" s="3">
         <v>15</v>
       </c>
-      <c r="R17">
+      <c r="U17" s="3">
         <v>6.18556701030928E-2</v>
       </c>
-      <c r="S17">
+      <c r="V17" s="3">
         <v>5.70342205323194E-2</v>
       </c>
-      <c r="T17" t="s">
-        <v>29</v>
-      </c>
-      <c r="U17" t="s">
-        <v>29</v>
-      </c>
-      <c r="V17" t="s">
-        <v>29</v>
-      </c>
-      <c r="W17" t="s">
-        <v>29</v>
-      </c>
-      <c r="X17" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y17" t="s">
+      <c r="W17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AC17" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="10">
         <v>43263</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F18">
+      <c r="I18" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G18" s="1">
+      <c r="J18" s="11">
         <v>43263.843344907407</v>
       </c>
-      <c r="H18">
+      <c r="K18" s="3">
         <v>1.5564819704297E-2</v>
       </c>
-      <c r="I18">
+      <c r="L18" s="3">
         <v>453</v>
       </c>
-      <c r="J18">
+      <c r="M18" s="3">
         <v>7.0508633260465201</v>
       </c>
-      <c r="K18" s="1">
+      <c r="N18" s="11">
         <v>43263.871527777781</v>
       </c>
-      <c r="L18" s="1">
+      <c r="O18" s="11">
         <v>43264.083333333336</v>
       </c>
-      <c r="M18" s="1">
+      <c r="P18" s="11">
         <v>43264.06417824074</v>
       </c>
-      <c r="N18">
+      <c r="Q18" s="3">
         <v>305</v>
       </c>
-      <c r="O18">
+      <c r="R18" s="3">
         <v>277</v>
       </c>
-      <c r="P18">
+      <c r="S18" s="3">
         <v>43</v>
       </c>
-      <c r="Q18">
+      <c r="T18" s="3">
         <v>35</v>
       </c>
-      <c r="R18">
+      <c r="U18" s="3">
         <v>0.14098360655737699</v>
       </c>
-      <c r="S18">
+      <c r="V18" s="3">
         <v>0.12635379061371799</v>
       </c>
-      <c r="T18" t="s">
-        <v>29</v>
-      </c>
-      <c r="U18" t="s">
-        <v>29</v>
-      </c>
-      <c r="V18" t="s">
-        <v>29</v>
-      </c>
-      <c r="W18" t="s">
-        <v>29</v>
-      </c>
-      <c r="X18" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y18" t="s">
+      <c r="W18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AC18" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="10">
         <v>43264</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F19">
+      <c r="I19" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G19" s="1">
+      <c r="J19" s="11">
         <v>43264.843622685185</v>
       </c>
-      <c r="H19">
+      <c r="K19" s="3">
         <v>1.2176310525898299E-3</v>
       </c>
-      <c r="I19">
+      <c r="L19" s="3">
         <v>395</v>
       </c>
-      <c r="J19">
+      <c r="M19" s="3">
         <v>0.48096426577298401</v>
       </c>
-      <c r="K19" s="1">
+      <c r="N19" s="11">
         <v>43264.870138888888</v>
       </c>
-      <c r="L19" s="1">
+      <c r="O19" s="11">
         <v>43265.083333333336</v>
       </c>
-      <c r="M19" s="1">
+      <c r="P19" s="11">
         <v>43265.064456018517</v>
       </c>
-      <c r="N19">
+      <c r="Q19" s="3">
         <v>307</v>
       </c>
-      <c r="O19">
+      <c r="R19" s="3">
         <v>279</v>
       </c>
-      <c r="P19">
+      <c r="S19" s="3">
         <v>14</v>
       </c>
-      <c r="Q19">
+      <c r="T19" s="3">
         <v>13</v>
       </c>
-      <c r="R19">
+      <c r="U19" s="3">
         <v>4.5602605863192203E-2</v>
       </c>
-      <c r="S19">
+      <c r="V19" s="3">
         <v>4.6594982078853001E-2</v>
       </c>
-      <c r="T19" t="s">
-        <v>29</v>
-      </c>
-      <c r="U19" t="s">
-        <v>29</v>
-      </c>
-      <c r="V19" t="s">
-        <v>29</v>
-      </c>
-      <c r="W19" t="s">
-        <v>29</v>
-      </c>
-      <c r="X19" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y19" t="s">
+      <c r="W19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AC19" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="10">
         <v>43291</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F20">
+      <c r="I20" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G20" s="1">
+      <c r="J20" s="11">
         <v>43291.844710648147</v>
       </c>
-      <c r="H20">
+      <c r="K20" s="3">
         <v>7.9329096396131393E-2</v>
       </c>
-      <c r="I20">
+      <c r="L20" s="3">
         <v>456</v>
       </c>
-      <c r="J20">
+      <c r="M20" s="3">
         <v>36.174067956635902</v>
       </c>
-      <c r="K20" s="1">
+      <c r="N20" s="11">
         <v>43291.866666666669</v>
       </c>
-      <c r="L20" s="1">
+      <c r="O20" s="11">
         <v>43292.086805555555</v>
       </c>
-      <c r="M20" s="1">
+      <c r="P20" s="11">
         <v>43292.06554398148</v>
       </c>
-      <c r="N20">
+      <c r="Q20" s="3">
         <v>317</v>
       </c>
-      <c r="O20">
+      <c r="R20" s="3">
         <v>286</v>
       </c>
-      <c r="P20">
+      <c r="S20" s="3">
         <v>11</v>
       </c>
-      <c r="Q20">
+      <c r="T20" s="3">
         <v>10</v>
       </c>
-      <c r="R20">
+      <c r="U20" s="3">
         <v>3.47003154574132E-2</v>
       </c>
-      <c r="S20">
+      <c r="V20" s="3">
         <v>3.4965034965035002E-2</v>
       </c>
-      <c r="T20" t="s">
-        <v>29</v>
-      </c>
-      <c r="U20" t="s">
-        <v>29</v>
-      </c>
-      <c r="V20" t="s">
-        <v>29</v>
-      </c>
-      <c r="W20" t="s">
-        <v>29</v>
-      </c>
-      <c r="X20" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y20" t="s">
+      <c r="W20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AC20" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="10">
         <v>43292</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F21">
+      <c r="I21" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G21" s="1">
+      <c r="J21" s="11">
         <v>43292.844490740739</v>
       </c>
-      <c r="H21">
+      <c r="K21" s="3">
         <v>2.4817719757652401E-2</v>
       </c>
-      <c r="I21">
+      <c r="L21" s="3">
         <v>421</v>
       </c>
-      <c r="J21">
+      <c r="M21" s="3">
         <v>10.448260017971601</v>
       </c>
-      <c r="K21" s="1">
+      <c r="N21" s="11">
         <v>43292.861111111109</v>
       </c>
-      <c r="L21" s="1">
+      <c r="O21" s="11">
         <v>43293.084722222222</v>
       </c>
-      <c r="M21" s="1">
+      <c r="P21" s="11">
         <v>43293.065324074072</v>
       </c>
-      <c r="N21">
+      <c r="Q21" s="3">
         <v>322</v>
       </c>
-      <c r="O21">
+      <c r="R21" s="3">
         <v>294</v>
       </c>
-      <c r="P21">
+      <c r="S21" s="3">
         <v>4</v>
       </c>
-      <c r="Q21">
+      <c r="T21" s="3">
         <v>4</v>
       </c>
-      <c r="R21">
+      <c r="U21" s="3">
         <v>1.2422360248447201E-2</v>
       </c>
-      <c r="S21">
+      <c r="V21" s="3">
         <v>1.3605442176870699E-2</v>
       </c>
-      <c r="T21" t="s">
-        <v>29</v>
-      </c>
-      <c r="U21" t="s">
-        <v>29</v>
-      </c>
-      <c r="V21" t="s">
-        <v>29</v>
-      </c>
-      <c r="W21" t="s">
-        <v>29</v>
-      </c>
-      <c r="X21" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y21" t="s">
+      <c r="W21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AC21" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="10">
         <v>43321</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F22">
+      <c r="I22" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G22" s="1">
+      <c r="J22" s="11">
         <v>43321.830879629626</v>
       </c>
-      <c r="H22">
+      <c r="K22" s="3">
         <v>3.7601778418734799E-2</v>
       </c>
-      <c r="I22">
+      <c r="L22" s="3">
         <v>428</v>
       </c>
-      <c r="J22">
+      <c r="M22" s="3">
         <v>16.093561163218499</v>
       </c>
-      <c r="K22" s="1">
+      <c r="N22" s="11">
         <v>43321.861111111109</v>
       </c>
-      <c r="L22" s="1">
+      <c r="O22" s="11">
         <v>43322.084027777775</v>
       </c>
-      <c r="M22" s="1">
+      <c r="P22" s="11">
         <v>43322.051712962966</v>
       </c>
-      <c r="N22">
+      <c r="Q22" s="3">
         <v>321</v>
       </c>
-      <c r="O22">
+      <c r="R22" s="3">
         <v>274</v>
       </c>
-      <c r="P22">
+      <c r="S22" s="3">
         <v>37</v>
       </c>
-      <c r="Q22">
+      <c r="T22" s="3">
         <v>35</v>
       </c>
-      <c r="R22">
+      <c r="U22" s="3">
         <v>0.11526479750778799</v>
       </c>
-      <c r="S22">
+      <c r="V22" s="3">
         <v>0.127737226277372</v>
       </c>
-      <c r="T22" t="s">
-        <v>29</v>
-      </c>
-      <c r="U22" t="s">
-        <v>29</v>
-      </c>
-      <c r="V22" t="s">
-        <v>29</v>
-      </c>
-      <c r="W22" t="s">
-        <v>29</v>
-      </c>
-      <c r="X22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y22" t="s">
+      <c r="W22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AC22" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="10">
         <v>43322</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2</v>
+      </c>
+      <c r="H23" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F23">
+      <c r="I23" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G23" s="1">
+      <c r="J23" s="11">
         <v>43322.83017361111</v>
       </c>
-      <c r="H23">
+      <c r="K23" s="3">
         <v>4.8051774331328697E-3</v>
       </c>
-      <c r="I23">
+      <c r="L23" s="3">
         <v>392</v>
       </c>
-      <c r="J23">
+      <c r="M23" s="3">
         <v>1.8836295537880801</v>
       </c>
-      <c r="K23" s="1">
+      <c r="N23" s="11">
         <v>43322.851388888892</v>
       </c>
-      <c r="L23" s="1">
+      <c r="O23" s="11">
         <v>43323.083333333336</v>
       </c>
-      <c r="M23" s="1">
+      <c r="P23" s="11">
         <v>43323.051006944443</v>
       </c>
-      <c r="N23">
+      <c r="Q23" s="3">
         <v>334</v>
       </c>
-      <c r="O23">
+      <c r="R23" s="3">
         <v>287</v>
       </c>
-      <c r="P23">
+      <c r="S23" s="3">
         <v>22</v>
       </c>
-      <c r="Q23">
+      <c r="T23" s="3">
         <v>20</v>
       </c>
-      <c r="R23">
+      <c r="U23" s="3">
         <v>6.5868263473053898E-2</v>
       </c>
-      <c r="S23">
+      <c r="V23" s="3">
         <v>6.9686411149825794E-2</v>
       </c>
-      <c r="T23" t="s">
-        <v>29</v>
-      </c>
-      <c r="U23" t="s">
-        <v>29</v>
-      </c>
-      <c r="V23" t="s">
-        <v>29</v>
-      </c>
-      <c r="W23" t="s">
-        <v>29</v>
-      </c>
-      <c r="X23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y23" t="s">
+      <c r="W23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="AC23" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="10">
         <v>43323</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" t="s">
+        <v>145</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+      <c r="H24" s="3">
         <v>34.056322999999999</v>
       </c>
-      <c r="F24">
+      <c r="I24" s="3">
         <v>-120.332024</v>
       </c>
-      <c r="G24" s="1">
+      <c r="J24" s="11">
         <v>43323.829467592594</v>
       </c>
-      <c r="H24">
+      <c r="K24" s="3">
         <v>3.1131241015873602E-3</v>
       </c>
-      <c r="I24">
+      <c r="L24" s="3">
         <v>441</v>
       </c>
-      <c r="J24">
+      <c r="M24" s="3">
         <v>1.3728877288000201</v>
       </c>
-      <c r="K24" s="1">
+      <c r="N24" s="11">
         <v>43323.854166666664</v>
       </c>
-      <c r="L24" s="1">
+      <c r="O24" s="11">
         <v>43324.084722222222</v>
       </c>
-      <c r="M24" s="1">
+      <c r="P24" s="11">
         <v>43324.050300925926</v>
       </c>
-      <c r="N24">
+      <c r="Q24" s="3">
         <v>332</v>
       </c>
-      <c r="O24">
+      <c r="R24" s="3">
         <v>282</v>
       </c>
-      <c r="P24">
+      <c r="S24" s="3">
         <v>11</v>
       </c>
-      <c r="Q24">
+      <c r="T24" s="3">
         <v>10</v>
       </c>
-      <c r="R24">
+      <c r="U24" s="3">
         <v>3.3132530120481903E-2</v>
       </c>
-      <c r="S24">
+      <c r="V24" s="3">
         <v>3.54609929078014E-2</v>
       </c>
-      <c r="T24" t="s">
-        <v>29</v>
-      </c>
-      <c r="U24" t="s">
-        <v>29</v>
-      </c>
-      <c r="V24" t="s">
-        <v>29</v>
-      </c>
-      <c r="W24" t="s">
-        <v>29</v>
-      </c>
-      <c r="X24" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y24" t="s">
+      <c r="W24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AC24" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="10">
         <v>42905</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F25">
+      <c r="I25" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G25" s="1">
+      <c r="J25" s="11">
         <v>42905.842789351853</v>
       </c>
-      <c r="H25">
+      <c r="K25" s="3">
         <v>0.25977860153252003</v>
       </c>
-      <c r="I25">
+      <c r="L25" s="3">
         <v>652</v>
       </c>
-      <c r="J25">
+      <c r="M25" s="3">
         <v>169.375648199203</v>
       </c>
-      <c r="K25" s="1">
+      <c r="N25" s="11">
         <v>42905.878472222219</v>
       </c>
-      <c r="L25" s="1">
+      <c r="O25" s="11">
         <v>42906.086805555555</v>
       </c>
-      <c r="M25" s="1">
+      <c r="P25" s="11">
         <v>42906.063622685186</v>
       </c>
-      <c r="N25">
+      <c r="Q25" s="3">
         <v>300</v>
       </c>
-      <c r="O25">
+      <c r="R25" s="3">
         <v>266</v>
       </c>
-      <c r="P25">
+      <c r="S25" s="3">
         <v>26</v>
       </c>
-      <c r="Q25">
+      <c r="T25" s="3">
         <v>23</v>
       </c>
-      <c r="R25">
+      <c r="U25" s="3">
         <v>8.6666666666666697E-2</v>
       </c>
-      <c r="S25">
+      <c r="V25" s="3">
         <v>8.6466165413533802E-2</v>
       </c>
-      <c r="T25" t="s">
+      <c r="W25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U25" t="s">
+      <c r="X25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V25" t="s">
+      <c r="Y25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W25" t="s">
+      <c r="Z25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X25" t="s">
+      <c r="AA25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="AB25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="AC25" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="10">
         <v>42906</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F26">
+      <c r="I26" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G26" s="1">
+      <c r="J26" s="11">
         <v>42906.842951388891</v>
       </c>
-      <c r="H26">
+      <c r="K26" s="3">
         <v>0.160452106148398</v>
       </c>
-      <c r="I26">
+      <c r="L26" s="3">
         <v>583</v>
       </c>
-      <c r="J26">
+      <c r="M26" s="3">
         <v>93.543577884515997</v>
       </c>
-      <c r="K26" s="1">
+      <c r="N26" s="11">
         <v>42906.885416666664</v>
       </c>
-      <c r="L26" s="1">
+      <c r="O26" s="11">
         <v>42907</v>
       </c>
-      <c r="M26" s="1">
+      <c r="P26" s="11">
         <v>42907.063784722224</v>
       </c>
-      <c r="N26">
+      <c r="Q26" s="3">
         <v>165</v>
       </c>
-      <c r="O26">
+      <c r="R26" s="3">
         <v>165</v>
       </c>
-      <c r="P26">
+      <c r="S26" s="3">
         <v>8</v>
       </c>
-      <c r="Q26">
+      <c r="T26" s="3">
         <v>8</v>
       </c>
-      <c r="R26">
+      <c r="U26" s="3">
         <v>4.8484848484848499E-2</v>
       </c>
-      <c r="S26">
+      <c r="V26" s="3">
         <v>4.8484848484848499E-2</v>
       </c>
-      <c r="T26" t="s">
+      <c r="W26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U26" t="s">
+      <c r="X26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V26" t="s">
+      <c r="Y26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W26" t="s">
+      <c r="Z26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X26" t="s">
+      <c r="AA26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="AB26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z26" t="s">
+      <c r="AC26" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="10">
         <v>42967</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F27">
+      <c r="I27" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G27" s="1">
+      <c r="J27" s="11">
         <v>42967.820104166669</v>
       </c>
-      <c r="H27">
+      <c r="K27" s="3">
         <v>1.15891693949371E-2</v>
       </c>
-      <c r="I27">
+      <c r="L27" s="3">
         <v>430</v>
       </c>
-      <c r="J27">
+      <c r="M27" s="3">
         <v>4.98334283982296</v>
       </c>
-      <c r="K27" s="1">
+      <c r="N27" s="11">
         <v>42967.859027777777</v>
       </c>
-      <c r="L27" s="1">
+      <c r="O27" s="11">
         <v>42968.083333333336</v>
       </c>
-      <c r="M27" s="1">
+      <c r="P27" s="11">
         <v>42968.040937500002</v>
       </c>
-      <c r="N27">
+      <c r="Q27" s="3">
         <v>323</v>
       </c>
-      <c r="O27">
+      <c r="R27" s="3">
         <v>261</v>
       </c>
-      <c r="P27">
+      <c r="S27" s="3">
         <v>6</v>
       </c>
-      <c r="Q27">
+      <c r="T27" s="3">
         <v>6</v>
       </c>
-      <c r="R27">
+      <c r="U27" s="3">
         <v>1.8575851393188899E-2</v>
       </c>
-      <c r="S27">
+      <c r="V27" s="3">
         <v>2.2988505747126398E-2</v>
       </c>
-      <c r="T27" t="s">
+      <c r="W27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U27" t="s">
+      <c r="X27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V27" t="s">
+      <c r="Y27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W27" t="s">
+      <c r="Z27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X27" t="s">
+      <c r="AA27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="AB27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AC27" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="10">
         <v>43262</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F28">
+      <c r="I28" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G28" s="1">
+      <c r="J28" s="11">
         <v>43262.840868055559</v>
       </c>
-      <c r="H28">
+      <c r="K28" s="3">
         <v>5.7667333922654003E-2</v>
       </c>
-      <c r="I28">
+      <c r="L28" s="3">
         <v>521</v>
       </c>
-      <c r="J28">
+      <c r="M28" s="3">
         <v>30.0446809737027</v>
       </c>
-      <c r="K28" s="1">
+      <c r="N28" s="11">
         <v>43262.88958333333</v>
       </c>
-      <c r="L28" s="1">
+      <c r="O28" s="11">
         <v>43263.083333333336</v>
       </c>
-      <c r="M28" s="1">
+      <c r="P28" s="11">
         <v>43263.061701388891</v>
       </c>
-      <c r="N28">
+      <c r="Q28" s="3">
         <v>279</v>
       </c>
-      <c r="O28">
+      <c r="R28" s="3">
         <v>247</v>
       </c>
-      <c r="P28">
+      <c r="S28" s="3">
         <v>32</v>
       </c>
-      <c r="Q28">
+      <c r="T28" s="3">
         <v>31</v>
       </c>
-      <c r="R28">
+      <c r="U28" s="3">
         <v>0.114695340501792</v>
       </c>
-      <c r="S28">
+      <c r="V28" s="3">
         <v>0.125506072874494</v>
       </c>
-      <c r="T28" t="s">
+      <c r="W28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U28" t="s">
+      <c r="X28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V28" t="s">
+      <c r="Y28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W28" t="s">
+      <c r="Z28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X28" t="s">
+      <c r="AA28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="AB28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z28" t="s">
+      <c r="AC28" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="10">
         <v>43263</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G29" s="3">
+        <v>2</v>
+      </c>
+      <c r="H29" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F29">
+      <c r="I29" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G29" s="1">
+      <c r="J29" s="11">
         <v>43263.841145833336</v>
       </c>
-      <c r="H29">
+      <c r="K29" s="3">
         <v>1.53133307699481E-2</v>
       </c>
-      <c r="I29">
+      <c r="L29" s="3">
         <v>445</v>
       </c>
-      <c r="J29">
+      <c r="M29" s="3">
         <v>6.8144321926269198</v>
       </c>
-      <c r="K29" s="1">
+      <c r="N29" s="11">
         <v>43263.875</v>
       </c>
-      <c r="L29" s="1">
+      <c r="O29" s="11">
         <v>43264.083333333336</v>
       </c>
-      <c r="M29" s="1">
+      <c r="P29" s="11">
         <v>43264.061979166669</v>
       </c>
-      <c r="N29">
+      <c r="Q29" s="3">
         <v>300</v>
       </c>
-      <c r="O29">
+      <c r="R29" s="3">
         <v>269</v>
       </c>
-      <c r="P29">
+      <c r="S29" s="3">
         <v>26</v>
       </c>
-      <c r="Q29">
+      <c r="T29" s="3">
         <v>25</v>
       </c>
-      <c r="R29">
+      <c r="U29" s="3">
         <v>8.6666666666666697E-2</v>
       </c>
-      <c r="S29">
+      <c r="V29" s="3">
         <v>9.2936802973977703E-2</v>
       </c>
-      <c r="T29" t="s">
+      <c r="W29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U29" t="s">
+      <c r="X29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V29" t="s">
+      <c r="Y29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W29" t="s">
+      <c r="Z29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X29" t="s">
+      <c r="AA29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="AB29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z29" t="s">
+      <c r="AC29" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="10">
         <v>43264</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" s="3">
+        <v>3</v>
+      </c>
+      <c r="H30" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F30">
+      <c r="I30" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G30" s="1">
+      <c r="J30" s="11">
         <v>43264.841423611113</v>
       </c>
-      <c r="H30">
+      <c r="K30" s="3">
         <v>1.12747454655941E-3</v>
       </c>
-      <c r="I30">
+      <c r="L30" s="3">
         <v>384</v>
       </c>
-      <c r="J30">
+      <c r="M30" s="3">
         <v>0.43295022587881199</v>
       </c>
-      <c r="K30" s="1">
+      <c r="N30" s="11">
         <v>43264.875</v>
       </c>
-      <c r="L30" s="1">
+      <c r="O30" s="11">
         <v>43265.084722222222</v>
       </c>
-      <c r="M30" s="1">
+      <c r="P30" s="11">
         <v>43265.062256944446</v>
       </c>
-      <c r="N30">
+      <c r="Q30" s="3">
         <v>302</v>
       </c>
-      <c r="O30">
+      <c r="R30" s="3">
         <v>269</v>
       </c>
-      <c r="P30">
+      <c r="S30" s="3">
         <v>13</v>
       </c>
-      <c r="Q30">
+      <c r="T30" s="3">
         <v>10</v>
       </c>
-      <c r="R30">
+      <c r="U30" s="3">
         <v>4.3046357615894003E-2</v>
       </c>
-      <c r="S30">
+      <c r="V30" s="3">
         <v>3.7174721189591101E-2</v>
       </c>
-      <c r="T30" t="s">
+      <c r="W30" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U30" t="s">
+      <c r="X30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V30" t="s">
+      <c r="Y30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W30" t="s">
+      <c r="Z30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X30" t="s">
+      <c r="AA30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="AB30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z30" t="s">
+      <c r="AC30" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="10">
         <v>43292</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F31">
+      <c r="I31" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G31" s="1">
+      <c r="J31" s="11">
         <v>43292.842303240737</v>
       </c>
-      <c r="H31">
+      <c r="K31" s="3">
         <v>2.47983022684004E-2</v>
       </c>
-      <c r="I31">
+      <c r="L31" s="3">
         <v>408</v>
       </c>
-      <c r="J31">
+      <c r="M31" s="3">
         <v>10.1177073255074</v>
       </c>
-      <c r="K31" s="1">
+      <c r="N31" s="11">
         <v>43292.875</v>
       </c>
-      <c r="L31" s="1">
+      <c r="O31" s="11">
         <v>43293.083333333336</v>
       </c>
-      <c r="M31" s="1">
+      <c r="P31" s="11">
         <v>43293.063136574077</v>
       </c>
-      <c r="N31">
+      <c r="Q31" s="3">
         <v>300</v>
       </c>
-      <c r="O31">
+      <c r="R31" s="3">
         <v>270</v>
       </c>
-      <c r="P31">
+      <c r="S31" s="3">
         <v>24</v>
       </c>
-      <c r="Q31">
+      <c r="T31" s="3">
         <v>21</v>
       </c>
-      <c r="R31">
+      <c r="U31" s="3">
         <v>0.08</v>
       </c>
-      <c r="S31">
+      <c r="V31" s="3">
         <v>7.7777777777777807E-2</v>
       </c>
-      <c r="T31" t="s">
+      <c r="W31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U31" t="s">
+      <c r="X31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V31" t="s">
+      <c r="Y31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W31" t="s">
+      <c r="Z31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X31" t="s">
+      <c r="AA31" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="AB31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z31" t="s">
+      <c r="AC31" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="10">
         <v>43318</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G32" s="3">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F32">
+      <c r="I32" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G32" s="1">
+      <c r="J32" s="11">
         <v>43318.830706018518</v>
       </c>
-      <c r="H32">
+      <c r="K32" s="3">
         <v>0.29163534604422398</v>
       </c>
-      <c r="I32">
+      <c r="L32" s="3">
         <v>468</v>
       </c>
-      <c r="J32">
+      <c r="M32" s="3">
         <v>136.485341948697</v>
       </c>
-      <c r="K32" s="1">
+      <c r="N32" s="11">
         <v>43318.920138888891</v>
       </c>
-      <c r="L32" s="1">
+      <c r="O32" s="11">
         <v>43319.085416666669</v>
       </c>
-      <c r="M32" s="1">
+      <c r="P32" s="11">
         <v>43319.051539351851</v>
       </c>
-      <c r="N32">
+      <c r="Q32" s="3">
         <v>238</v>
       </c>
-      <c r="O32">
+      <c r="R32" s="3">
         <v>189</v>
       </c>
-      <c r="P32">
+      <c r="S32" s="3">
         <v>6</v>
       </c>
-      <c r="Q32">
+      <c r="T32" s="3">
         <v>4</v>
       </c>
-      <c r="R32">
+      <c r="U32" s="3">
         <v>2.5210084033613401E-2</v>
       </c>
-      <c r="S32">
+      <c r="V32" s="3">
         <v>2.1164021164021201E-2</v>
       </c>
-      <c r="T32" t="s">
+      <c r="W32" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U32" t="s">
+      <c r="X32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V32" t="s">
+      <c r="Y32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W32" t="s">
+      <c r="Z32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X32" t="s">
+      <c r="AA32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="AB32" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AC32" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="10">
         <v>43320</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G33" s="13">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3">
         <v>34.047666</v>
       </c>
-      <c r="F33">
+      <c r="I33" s="3">
         <v>-119.547674</v>
       </c>
-      <c r="G33" s="1">
+      <c r="J33" s="11">
         <v>43320.829375000001</v>
       </c>
-      <c r="H33">
+      <c r="K33" s="3">
         <v>0.100925051886401</v>
       </c>
-      <c r="I33">
+      <c r="L33" s="3">
         <v>402</v>
       </c>
-      <c r="J33">
+      <c r="M33" s="3">
         <v>40.571870858333099</v>
       </c>
-      <c r="K33" s="1">
+      <c r="N33" s="11">
         <v>43320.876388888886</v>
       </c>
-      <c r="L33" s="1">
+      <c r="O33" s="11">
         <v>43321.083333333336</v>
       </c>
-      <c r="M33" s="1">
+      <c r="P33" s="11">
         <v>43321.050208333334</v>
       </c>
-      <c r="N33">
+      <c r="Q33" s="3">
         <v>298</v>
       </c>
-      <c r="O33">
+      <c r="R33" s="3">
         <v>250</v>
       </c>
-      <c r="P33">
+      <c r="S33" s="3">
         <v>10</v>
       </c>
-      <c r="Q33">
+      <c r="T33" s="3">
         <v>10</v>
       </c>
-      <c r="R33">
+      <c r="U33" s="3">
         <v>3.35570469798658E-2</v>
       </c>
-      <c r="S33">
+      <c r="V33" s="3">
         <v>0.04</v>
       </c>
-      <c r="T33" t="s">
+      <c r="W33" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U33" t="s">
+      <c r="X33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V33" t="s">
+      <c r="Y33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W33" t="s">
+      <c r="Z33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X33" t="s">
+      <c r="AA33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="AB33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z33" t="s">
+      <c r="AC33" s="3" t="s">
         <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
     <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>